<commit_message>
fix formatting issue in data
</commit_message>
<xml_diff>
--- a/archiveddata/shanghai-2014.xlsx
+++ b/archiveddata/shanghai-2014.xlsx
@@ -4,14 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23812"/>
   <workbookPr showInkAnnotation="0" checkCompatibility="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="4180" yWindow="1120" windowWidth="14400" windowHeight="16600" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
     <sheet name="工作表2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">工作表1!$A$1:$G$191</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">工作表1!$A$1:$F$191</definedName>
   </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1772" uniqueCount="1136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1579" uniqueCount="1130">
   <si>
     <t>序号</t>
   </si>
@@ -7214,37 +7214,13 @@
   </si>
   <si>
     <t>安全技术防范产品持证信息</t>
-  </si>
-  <si>
-    <t>已开放</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>已开放</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>未开放-5.8</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>疑似开放</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>备注</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>有早餐工程网点数据</t>
-    <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -7310,11 +7286,6 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="仿宋"/>
-    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -7330,7 +7301,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -7366,26 +7337,6 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -7394,7 +7345,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
@@ -7423,12 +7374,6 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="普通" xfId="0" builtinId="0"/>
@@ -7764,11 +7709,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A1:H191"/>
+  <dimension ref="A1:F191"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H30" sqref="H30"/>
+      <selection activeCell="G1" sqref="G1:H1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -7781,7 +7725,7 @@
     <col min="6" max="6" width="11.5" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="30">
+    <row r="1" spans="1:6" ht="30">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -7800,14 +7744,8 @@
       <c r="F1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="5" t="s">
-        <v>1130</v>
-      </c>
-      <c r="H1" s="12" t="s">
-        <v>1134</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="39" hidden="1">
+    </row>
+    <row r="2" spans="1:6" ht="39">
       <c r="A2" s="6" t="s">
         <v>5</v>
       </c>
@@ -7826,11 +7764,8 @@
       <c r="F2" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G2" t="s">
-        <v>1131</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="39" hidden="1">
+    </row>
+    <row r="3" spans="1:6" ht="39">
       <c r="A3" s="6" t="s">
         <v>11</v>
       </c>
@@ -7849,11 +7784,8 @@
       <c r="F3" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G3" t="s">
-        <v>1131</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="39" hidden="1">
+    </row>
+    <row r="4" spans="1:6" ht="39">
       <c r="A4" s="6" t="s">
         <v>15</v>
       </c>
@@ -7872,11 +7804,8 @@
       <c r="F4" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="G4" t="s">
-        <v>1131</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="52" hidden="1">
+    </row>
+    <row r="5" spans="1:6" ht="52">
       <c r="A5" s="6" t="s">
         <v>20</v>
       </c>
@@ -7895,11 +7824,8 @@
       <c r="F5" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="G5" t="s">
-        <v>1131</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="39" hidden="1">
+    </row>
+    <row r="6" spans="1:6" ht="39">
       <c r="A6" s="6" t="s">
         <v>24</v>
       </c>
@@ -7918,11 +7844,8 @@
       <c r="F6" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="G6" t="s">
-        <v>1131</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="65" hidden="1">
+    </row>
+    <row r="7" spans="1:6" ht="65">
       <c r="A7" s="6" t="s">
         <v>28</v>
       </c>
@@ -7941,11 +7864,8 @@
       <c r="F7" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="G7" t="s">
-        <v>1131</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="39" hidden="1">
+    </row>
+    <row r="8" spans="1:6" ht="39">
       <c r="A8" s="6" t="s">
         <v>32</v>
       </c>
@@ -7964,11 +7884,8 @@
       <c r="F8" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="G8" t="s">
-        <v>1131</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="52" hidden="1">
+    </row>
+    <row r="9" spans="1:6" ht="52">
       <c r="A9" s="6" t="s">
         <v>37</v>
       </c>
@@ -7987,11 +7904,8 @@
       <c r="F9" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="G9" t="s">
-        <v>1131</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="51" customHeight="1">
+    </row>
+    <row r="10" spans="1:6" ht="51" customHeight="1">
       <c r="A10" s="9" t="s">
         <v>41</v>
       </c>
@@ -8010,11 +7924,8 @@
       <c r="F10" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="G10" t="s">
-        <v>1132</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="52" hidden="1">
+    </row>
+    <row r="11" spans="1:6" ht="52">
       <c r="A11" s="6" t="s">
         <v>45</v>
       </c>
@@ -8033,11 +7944,8 @@
       <c r="F11" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="G11" t="s">
-        <v>1131</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="39" hidden="1">
+    </row>
+    <row r="12" spans="1:6" ht="39">
       <c r="A12" s="6" t="s">
         <v>49</v>
       </c>
@@ -8056,11 +7964,8 @@
       <c r="F12" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="G12" t="s">
-        <v>1131</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="39" hidden="1">
+    </row>
+    <row r="13" spans="1:6" ht="39">
       <c r="A13" s="6" t="s">
         <v>53</v>
       </c>
@@ -8079,11 +7984,8 @@
       <c r="F13" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="G13" t="s">
-        <v>1131</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="65" hidden="1">
+    </row>
+    <row r="14" spans="1:6" ht="65">
       <c r="A14" s="6" t="s">
         <v>57</v>
       </c>
@@ -8102,11 +8004,8 @@
       <c r="F14" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="G14" t="s">
-        <v>1131</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="65">
+    </row>
+    <row r="15" spans="1:6" ht="65">
       <c r="A15" s="6" t="s">
         <v>61</v>
       </c>
@@ -8125,11 +8024,8 @@
       <c r="F15" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="G15" t="s">
-        <v>1132</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="52">
+    </row>
+    <row r="16" spans="1:6" ht="52">
       <c r="A16" s="6" t="s">
         <v>65</v>
       </c>
@@ -8148,11 +8044,8 @@
       <c r="F16" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="G16" t="s">
-        <v>1132</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="39" hidden="1">
+    </row>
+    <row r="17" spans="1:6" ht="39">
       <c r="A17" s="6" t="s">
         <v>69</v>
       </c>
@@ -8171,11 +8064,8 @@
       <c r="F17" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="G17" t="s">
-        <v>1131</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="65" hidden="1">
+    </row>
+    <row r="18" spans="1:6" ht="65">
       <c r="A18" s="6" t="s">
         <v>72</v>
       </c>
@@ -8194,11 +8084,8 @@
       <c r="F18" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="G18" t="s">
-        <v>1131</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" ht="39" hidden="1">
+    </row>
+    <row r="19" spans="1:6" ht="39">
       <c r="A19" s="6" t="s">
         <v>76</v>
       </c>
@@ -8217,11 +8104,8 @@
       <c r="F19" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="G19" t="s">
-        <v>1131</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="52" hidden="1">
+    </row>
+    <row r="20" spans="1:6" ht="52">
       <c r="A20" s="6" t="s">
         <v>80</v>
       </c>
@@ -8240,11 +8124,8 @@
       <c r="F20" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="G20" t="s">
-        <v>1131</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" ht="65" hidden="1">
+    </row>
+    <row r="21" spans="1:6" ht="65">
       <c r="A21" s="6" t="s">
         <v>84</v>
       </c>
@@ -8263,11 +8144,8 @@
       <c r="F21" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="G21" t="s">
-        <v>1131</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" ht="39" hidden="1">
+    </row>
+    <row r="22" spans="1:6" ht="39">
       <c r="A22" s="6" t="s">
         <v>88</v>
       </c>
@@ -8286,11 +8164,8 @@
       <c r="F22" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="G22" t="s">
-        <v>1131</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" ht="39" hidden="1">
+    </row>
+    <row r="23" spans="1:6" ht="39">
       <c r="A23" s="6" t="s">
         <v>92</v>
       </c>
@@ -8309,11 +8184,8 @@
       <c r="F23" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="G23" t="s">
-        <v>1131</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" ht="26" hidden="1">
+    </row>
+    <row r="24" spans="1:6" ht="26">
       <c r="A24" s="6" t="s">
         <v>96</v>
       </c>
@@ -8332,11 +8204,8 @@
       <c r="F24" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="G24" t="s">
-        <v>1131</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" ht="39" hidden="1">
+    </row>
+    <row r="25" spans="1:6" ht="39">
       <c r="A25" s="6" t="s">
         <v>100</v>
       </c>
@@ -8355,11 +8224,8 @@
       <c r="F25" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G25" t="s">
-        <v>1131</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" ht="26" hidden="1">
+    </row>
+    <row r="26" spans="1:6" ht="26">
       <c r="A26" s="6" t="s">
         <v>104</v>
       </c>
@@ -8378,11 +8244,8 @@
       <c r="F26" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G26" t="s">
-        <v>1131</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" ht="39" hidden="1">
+    </row>
+    <row r="27" spans="1:6" ht="39">
       <c r="A27" s="6" t="s">
         <v>108</v>
       </c>
@@ -8401,11 +8264,8 @@
       <c r="F27" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G27" t="s">
-        <v>1131</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" ht="65" hidden="1">
+    </row>
+    <row r="28" spans="1:6" ht="65">
       <c r="A28" s="6" t="s">
         <v>112</v>
       </c>
@@ -8424,11 +8284,8 @@
       <c r="F28" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G28" t="s">
-        <v>1131</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" ht="49" customHeight="1">
+    </row>
+    <row r="29" spans="1:6" ht="49" customHeight="1">
       <c r="A29" s="9" t="s">
         <v>116</v>
       </c>
@@ -8447,14 +8304,8 @@
       <c r="F29" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="G29" t="s">
-        <v>1133</v>
-      </c>
-      <c r="H29" s="13" t="s">
-        <v>1135</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" ht="78">
+    </row>
+    <row r="30" spans="1:6" ht="78">
       <c r="A30" s="6" t="s">
         <v>121</v>
       </c>
@@ -8473,11 +8324,8 @@
       <c r="F30" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G30" t="s">
-        <v>1132</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" ht="39">
+    </row>
+    <row r="31" spans="1:6" ht="39">
       <c r="A31" s="6" t="s">
         <v>125</v>
       </c>
@@ -8496,11 +8344,8 @@
       <c r="F31" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G31" t="s">
-        <v>1132</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" ht="52">
+    </row>
+    <row r="32" spans="1:6" ht="52">
       <c r="A32" s="6" t="s">
         <v>129</v>
       </c>
@@ -8519,11 +8364,8 @@
       <c r="F32" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G32" t="s">
-        <v>1132</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" ht="91">
+    </row>
+    <row r="33" spans="1:6" ht="91">
       <c r="A33" s="6" t="s">
         <v>133</v>
       </c>
@@ -8542,11 +8384,8 @@
       <c r="F33" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="G33" t="s">
-        <v>1132</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" ht="39">
+    </row>
+    <row r="34" spans="1:6" ht="39">
       <c r="A34" s="6" t="s">
         <v>137</v>
       </c>
@@ -8565,11 +8404,8 @@
       <c r="F34" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="G34" t="s">
-        <v>1132</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" ht="65">
+    </row>
+    <row r="35" spans="1:6" ht="65">
       <c r="A35" s="6" t="s">
         <v>141</v>
       </c>
@@ -8588,11 +8424,8 @@
       <c r="F35" s="6" t="s">
         <v>146</v>
       </c>
-      <c r="G35" t="s">
-        <v>1132</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" ht="52">
+    </row>
+    <row r="36" spans="1:6" ht="52">
       <c r="A36" s="6" t="s">
         <v>147</v>
       </c>
@@ -8611,11 +8444,8 @@
       <c r="F36" s="6" t="s">
         <v>146</v>
       </c>
-      <c r="G36" t="s">
-        <v>1132</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" ht="52">
+    </row>
+    <row r="37" spans="1:6" ht="52">
       <c r="A37" s="6" t="s">
         <v>151</v>
       </c>
@@ -8634,11 +8464,8 @@
       <c r="F37" s="6" t="s">
         <v>146</v>
       </c>
-      <c r="G37" t="s">
-        <v>1132</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" ht="26">
+    </row>
+    <row r="38" spans="1:6" ht="26">
       <c r="A38" s="6" t="s">
         <v>155</v>
       </c>
@@ -8657,11 +8484,8 @@
       <c r="F38" s="6" t="s">
         <v>146</v>
       </c>
-      <c r="G38" t="s">
-        <v>1132</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" ht="26">
+    </row>
+    <row r="39" spans="1:6" ht="26">
       <c r="A39" s="6" t="s">
         <v>158</v>
       </c>
@@ -8680,11 +8504,8 @@
       <c r="F39" s="6" t="s">
         <v>146</v>
       </c>
-      <c r="G39" t="s">
-        <v>1132</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" ht="91">
+    </row>
+    <row r="40" spans="1:6" ht="91">
       <c r="A40" s="6" t="s">
         <v>161</v>
       </c>
@@ -8703,11 +8524,8 @@
       <c r="F40" s="6" t="s">
         <v>146</v>
       </c>
-      <c r="G40" t="s">
-        <v>1132</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" ht="39">
+    </row>
+    <row r="41" spans="1:6" ht="39">
       <c r="A41" s="6" t="s">
         <v>165</v>
       </c>
@@ -8726,11 +8544,8 @@
       <c r="F41" s="6" t="s">
         <v>146</v>
       </c>
-      <c r="G41" t="s">
-        <v>1132</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" ht="39">
+    </row>
+    <row r="42" spans="1:6" ht="39">
       <c r="A42" s="6" t="s">
         <v>169</v>
       </c>
@@ -8749,11 +8564,8 @@
       <c r="F42" s="6" t="s">
         <v>146</v>
       </c>
-      <c r="G42" t="s">
-        <v>1132</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" ht="52" hidden="1">
+    </row>
+    <row r="43" spans="1:6" ht="52">
       <c r="A43" s="6" t="s">
         <v>173</v>
       </c>
@@ -8772,11 +8584,8 @@
       <c r="F43" s="6" t="s">
         <v>146</v>
       </c>
-      <c r="G43" t="s">
-        <v>1131</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" ht="78" hidden="1">
+    </row>
+    <row r="44" spans="1:6" ht="78">
       <c r="A44" s="6" t="s">
         <v>178</v>
       </c>
@@ -8795,11 +8604,8 @@
       <c r="F44" s="6" t="s">
         <v>146</v>
       </c>
-      <c r="G44" t="s">
-        <v>1131</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" ht="52" hidden="1">
+    </row>
+    <row r="45" spans="1:6" ht="52">
       <c r="A45" s="6" t="s">
         <v>182</v>
       </c>
@@ -8818,11 +8624,8 @@
       <c r="F45" s="6" t="s">
         <v>146</v>
       </c>
-      <c r="G45" t="s">
-        <v>1131</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" ht="78" hidden="1">
+    </row>
+    <row r="46" spans="1:6" ht="78">
       <c r="A46" s="6" t="s">
         <v>185</v>
       </c>
@@ -8841,11 +8644,8 @@
       <c r="F46" s="6" t="s">
         <v>146</v>
       </c>
-      <c r="G46" t="s">
-        <v>1131</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" ht="52" hidden="1">
+    </row>
+    <row r="47" spans="1:6" ht="52">
       <c r="A47" s="6" t="s">
         <v>189</v>
       </c>
@@ -8864,11 +8664,8 @@
       <c r="F47" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G47" t="s">
-        <v>1131</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" ht="39" hidden="1">
+    </row>
+    <row r="48" spans="1:6" ht="39">
       <c r="A48" s="6" t="s">
         <v>194</v>
       </c>
@@ -8887,11 +8684,8 @@
       <c r="F48" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G48" t="s">
-        <v>1131</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" ht="52" hidden="1">
+    </row>
+    <row r="49" spans="1:6" ht="52">
       <c r="A49" s="6" t="s">
         <v>198</v>
       </c>
@@ -8910,11 +8704,8 @@
       <c r="F49" s="6" t="s">
         <v>202</v>
       </c>
-      <c r="G49" t="s">
-        <v>1131</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" ht="39">
+    </row>
+    <row r="50" spans="1:6" ht="39">
       <c r="A50" s="6" t="s">
         <v>203</v>
       </c>
@@ -8933,11 +8724,8 @@
       <c r="F50" s="6" t="s">
         <v>202</v>
       </c>
-      <c r="G50" t="s">
-        <v>1132</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" ht="52">
+    </row>
+    <row r="51" spans="1:6" ht="52">
       <c r="A51" s="6" t="s">
         <v>207</v>
       </c>
@@ -8956,11 +8744,8 @@
       <c r="F51" s="6" t="s">
         <v>202</v>
       </c>
-      <c r="G51" t="s">
-        <v>1132</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" ht="52">
+    </row>
+    <row r="52" spans="1:6" ht="52">
       <c r="A52" s="6" t="s">
         <v>211</v>
       </c>
@@ -8979,11 +8764,8 @@
       <c r="F52" s="6" t="s">
         <v>202</v>
       </c>
-      <c r="G52" t="s">
-        <v>1132</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" ht="52">
+    </row>
+    <row r="53" spans="1:6" ht="52">
       <c r="A53" s="6" t="s">
         <v>214</v>
       </c>
@@ -9002,11 +8784,8 @@
       <c r="F53" s="6" t="s">
         <v>202</v>
       </c>
-      <c r="G53" t="s">
-        <v>1132</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" ht="65">
+    </row>
+    <row r="54" spans="1:6" ht="65">
       <c r="A54" s="6" t="s">
         <v>218</v>
       </c>
@@ -9025,11 +8804,8 @@
       <c r="F54" s="6" t="s">
         <v>202</v>
       </c>
-      <c r="G54" t="s">
-        <v>1132</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" ht="39">
+    </row>
+    <row r="55" spans="1:6" ht="39">
       <c r="A55" s="6" t="s">
         <v>222</v>
       </c>
@@ -9048,11 +8824,8 @@
       <c r="F55" s="6" t="s">
         <v>202</v>
       </c>
-      <c r="G55" t="s">
-        <v>1132</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" ht="52" hidden="1">
+    </row>
+    <row r="56" spans="1:6" ht="52">
       <c r="A56" s="6" t="s">
         <v>226</v>
       </c>
@@ -9071,11 +8844,8 @@
       <c r="F56" s="6" t="s">
         <v>202</v>
       </c>
-      <c r="G56" t="s">
-        <v>1131</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" ht="41" customHeight="1">
+    </row>
+    <row r="57" spans="1:6" ht="41" customHeight="1">
       <c r="A57" s="9" t="s">
         <v>230</v>
       </c>
@@ -9094,11 +8864,8 @@
       <c r="F57" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="G57" t="s">
-        <v>1132</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" ht="78">
+    </row>
+    <row r="58" spans="1:6" ht="78">
       <c r="A58" s="6" t="s">
         <v>235</v>
       </c>
@@ -9117,11 +8884,8 @@
       <c r="F58" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G58" t="s">
-        <v>1132</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" ht="52">
+    </row>
+    <row r="59" spans="1:6" ht="52">
       <c r="A59" s="6" t="s">
         <v>238</v>
       </c>
@@ -9140,11 +8904,8 @@
       <c r="F59" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G59" t="s">
-        <v>1132</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" ht="39">
+    </row>
+    <row r="60" spans="1:6" ht="39">
       <c r="A60" s="6" t="s">
         <v>241</v>
       </c>
@@ -9163,11 +8924,8 @@
       <c r="F60" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G60" t="s">
-        <v>1132</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7" ht="91">
+    </row>
+    <row r="61" spans="1:6" ht="91">
       <c r="A61" s="6" t="s">
         <v>244</v>
       </c>
@@ -9186,11 +8944,8 @@
       <c r="F61" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G61" t="s">
-        <v>1132</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7" ht="91">
+    </row>
+    <row r="62" spans="1:6" ht="91">
       <c r="A62" s="6" t="s">
         <v>247</v>
       </c>
@@ -9209,11 +8964,8 @@
       <c r="F62" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G62" t="s">
-        <v>1132</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7" ht="78">
+    </row>
+    <row r="63" spans="1:6" ht="78">
       <c r="A63" s="6" t="s">
         <v>251</v>
       </c>
@@ -9232,11 +8984,8 @@
       <c r="F63" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G63" t="s">
-        <v>1132</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7" ht="39">
+    </row>
+    <row r="64" spans="1:6" ht="39">
       <c r="A64" s="6" t="s">
         <v>256</v>
       </c>
@@ -9255,11 +9004,8 @@
       <c r="F64" s="6" t="s">
         <v>261</v>
       </c>
-      <c r="G64" t="s">
-        <v>1132</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7" ht="52">
+    </row>
+    <row r="65" spans="1:6" ht="52">
       <c r="A65" s="6" t="s">
         <v>262</v>
       </c>
@@ -9278,11 +9024,8 @@
       <c r="F65" s="6" t="s">
         <v>261</v>
       </c>
-      <c r="G65" t="s">
-        <v>1132</v>
-      </c>
-    </row>
-    <row r="66" spans="1:7" ht="52" hidden="1">
+    </row>
+    <row r="66" spans="1:6" ht="52">
       <c r="A66" s="6" t="s">
         <v>266</v>
       </c>
@@ -9301,11 +9044,8 @@
       <c r="F66" s="6" t="s">
         <v>261</v>
       </c>
-      <c r="G66" t="s">
-        <v>1131</v>
-      </c>
-    </row>
-    <row r="67" spans="1:7" ht="52" hidden="1">
+    </row>
+    <row r="67" spans="1:6" ht="52">
       <c r="A67" s="6" t="s">
         <v>270</v>
       </c>
@@ -9324,11 +9064,8 @@
       <c r="F67" s="6" t="s">
         <v>261</v>
       </c>
-      <c r="G67" t="s">
-        <v>1131</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7" ht="78" hidden="1">
+    </row>
+    <row r="68" spans="1:6" ht="78">
       <c r="A68" s="6" t="s">
         <v>274</v>
       </c>
@@ -9347,11 +9084,8 @@
       <c r="F68" s="6" t="s">
         <v>261</v>
       </c>
-      <c r="G68" t="s">
-        <v>1131</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7" ht="52">
+    </row>
+    <row r="69" spans="1:6" ht="52">
       <c r="A69" s="6" t="s">
         <v>278</v>
       </c>
@@ -9370,11 +9104,8 @@
       <c r="F69" s="6" t="s">
         <v>261</v>
       </c>
-      <c r="G69" t="s">
-        <v>1132</v>
-      </c>
-    </row>
-    <row r="70" spans="1:7" ht="39" hidden="1">
+    </row>
+    <row r="70" spans="1:6" ht="39">
       <c r="A70" s="6" t="s">
         <v>282</v>
       </c>
@@ -9393,11 +9124,8 @@
       <c r="F70" s="6" t="s">
         <v>261</v>
       </c>
-      <c r="G70" t="s">
-        <v>1131</v>
-      </c>
-    </row>
-    <row r="71" spans="1:7" ht="39">
+    </row>
+    <row r="71" spans="1:6" ht="39">
       <c r="A71" s="6" t="s">
         <v>285</v>
       </c>
@@ -9416,11 +9144,8 @@
       <c r="F71" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G71" t="s">
-        <v>1132</v>
-      </c>
-    </row>
-    <row r="72" spans="1:7" ht="39">
+    </row>
+    <row r="72" spans="1:6" ht="39">
       <c r="A72" s="6" t="s">
         <v>290</v>
       </c>
@@ -9439,11 +9164,8 @@
       <c r="F72" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G72" t="s">
-        <v>1132</v>
-      </c>
-    </row>
-    <row r="73" spans="1:7" ht="52">
+    </row>
+    <row r="73" spans="1:6" ht="52">
       <c r="A73" s="6" t="s">
         <v>293</v>
       </c>
@@ -9462,11 +9184,8 @@
       <c r="F73" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G73" t="s">
-        <v>1132</v>
-      </c>
-    </row>
-    <row r="74" spans="1:7" ht="39">
+    </row>
+    <row r="74" spans="1:6" ht="39">
       <c r="A74" s="6" t="s">
         <v>297</v>
       </c>
@@ -9485,11 +9204,8 @@
       <c r="F74" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G74" t="s">
-        <v>1132</v>
-      </c>
-    </row>
-    <row r="75" spans="1:7" ht="39">
+    </row>
+    <row r="75" spans="1:6" ht="39">
       <c r="A75" s="6" t="s">
         <v>300</v>
       </c>
@@ -9508,11 +9224,8 @@
       <c r="F75" s="6" t="s">
         <v>304</v>
       </c>
-      <c r="G75" t="s">
-        <v>1132</v>
-      </c>
-    </row>
-    <row r="76" spans="1:7" ht="39">
+    </row>
+    <row r="76" spans="1:6" ht="39">
       <c r="A76" s="6" t="s">
         <v>305</v>
       </c>
@@ -9531,11 +9244,8 @@
       <c r="F76" s="6" t="s">
         <v>309</v>
       </c>
-      <c r="G76" t="s">
-        <v>1132</v>
-      </c>
-    </row>
-    <row r="77" spans="1:7" ht="39">
+    </row>
+    <row r="77" spans="1:6" ht="39">
       <c r="A77" s="6" t="s">
         <v>310</v>
       </c>
@@ -9554,11 +9264,8 @@
       <c r="F77" s="6" t="s">
         <v>309</v>
       </c>
-      <c r="G77" t="s">
-        <v>1132</v>
-      </c>
-    </row>
-    <row r="78" spans="1:7" ht="39">
+    </row>
+    <row r="78" spans="1:6" ht="39">
       <c r="A78" s="6" t="s">
         <v>314</v>
       </c>
@@ -9577,11 +9284,8 @@
       <c r="F78" s="6" t="s">
         <v>309</v>
       </c>
-      <c r="G78" t="s">
-        <v>1132</v>
-      </c>
-    </row>
-    <row r="79" spans="1:7" ht="39">
+    </row>
+    <row r="79" spans="1:6" ht="39">
       <c r="A79" s="6" t="s">
         <v>317</v>
       </c>
@@ -9600,11 +9304,8 @@
       <c r="F79" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G79" t="s">
-        <v>1132</v>
-      </c>
-    </row>
-    <row r="80" spans="1:7" ht="65">
+    </row>
+    <row r="80" spans="1:6" ht="65">
       <c r="A80" s="6" t="s">
         <v>322</v>
       </c>
@@ -9623,11 +9324,8 @@
       <c r="F80" s="6" t="s">
         <v>326</v>
       </c>
-      <c r="G80" t="s">
-        <v>1132</v>
-      </c>
-    </row>
-    <row r="81" spans="1:7" ht="39">
+    </row>
+    <row r="81" spans="1:6" ht="39">
       <c r="A81" s="6" t="s">
         <v>327</v>
       </c>
@@ -9646,11 +9344,8 @@
       <c r="F81" s="6" t="s">
         <v>202</v>
       </c>
-      <c r="G81" t="s">
-        <v>1132</v>
-      </c>
-    </row>
-    <row r="82" spans="1:7" ht="39">
+    </row>
+    <row r="82" spans="1:6" ht="39">
       <c r="A82" s="6" t="s">
         <v>332</v>
       </c>
@@ -9669,11 +9364,8 @@
       <c r="F82" s="6" t="s">
         <v>202</v>
       </c>
-      <c r="G82" t="s">
-        <v>1132</v>
-      </c>
-    </row>
-    <row r="83" spans="1:7" ht="39">
+    </row>
+    <row r="83" spans="1:6" ht="39">
       <c r="A83" s="6" t="s">
         <v>336</v>
       </c>
@@ -9692,11 +9384,8 @@
       <c r="F83" s="6" t="s">
         <v>202</v>
       </c>
-      <c r="G83" t="s">
-        <v>1132</v>
-      </c>
-    </row>
-    <row r="84" spans="1:7" ht="78">
+    </row>
+    <row r="84" spans="1:6" ht="78">
       <c r="A84" s="6" t="s">
         <v>340</v>
       </c>
@@ -9715,11 +9404,8 @@
       <c r="F84" s="6" t="s">
         <v>202</v>
       </c>
-      <c r="G84" t="s">
-        <v>1132</v>
-      </c>
-    </row>
-    <row r="85" spans="1:7" ht="39" hidden="1">
+    </row>
+    <row r="85" spans="1:6" ht="39">
       <c r="A85" s="6" t="s">
         <v>344</v>
       </c>
@@ -9738,11 +9424,8 @@
       <c r="F85" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G85" t="s">
-        <v>1131</v>
-      </c>
-    </row>
-    <row r="86" spans="1:7" ht="52" hidden="1">
+    </row>
+    <row r="86" spans="1:6" ht="52">
       <c r="A86" s="6" t="s">
         <v>348</v>
       </c>
@@ -9761,11 +9444,8 @@
       <c r="F86" s="6" t="s">
         <v>202</v>
       </c>
-      <c r="G86" t="s">
-        <v>1131</v>
-      </c>
-    </row>
-    <row r="87" spans="1:7" ht="39">
+    </row>
+    <row r="87" spans="1:6" ht="39">
       <c r="A87" s="6" t="s">
         <v>352</v>
       </c>
@@ -9784,11 +9464,8 @@
       <c r="F87" s="6" t="s">
         <v>202</v>
       </c>
-      <c r="G87" t="s">
-        <v>1132</v>
-      </c>
-    </row>
-    <row r="88" spans="1:7" ht="52" hidden="1">
+    </row>
+    <row r="88" spans="1:6" ht="52">
       <c r="A88" s="6" t="s">
         <v>356</v>
       </c>
@@ -9807,11 +9484,8 @@
       <c r="F88" s="6" t="s">
         <v>202</v>
       </c>
-      <c r="G88" t="s">
-        <v>1131</v>
-      </c>
-    </row>
-    <row r="89" spans="1:7" ht="26">
+    </row>
+    <row r="89" spans="1:6" ht="26">
       <c r="A89" s="6" t="s">
         <v>360</v>
       </c>
@@ -9830,11 +9504,8 @@
       <c r="F89" s="6" t="s">
         <v>326</v>
       </c>
-      <c r="G89" t="s">
-        <v>1132</v>
-      </c>
-    </row>
-    <row r="90" spans="1:7" ht="52" hidden="1">
+    </row>
+    <row r="90" spans="1:6" ht="52">
       <c r="A90" s="6" t="s">
         <v>364</v>
       </c>
@@ -9853,11 +9524,8 @@
       <c r="F90" s="6" t="s">
         <v>202</v>
       </c>
-      <c r="G90" t="s">
-        <v>1131</v>
-      </c>
-    </row>
-    <row r="91" spans="1:7" ht="52">
+    </row>
+    <row r="91" spans="1:6" ht="52">
       <c r="A91" s="6" t="s">
         <v>369</v>
       </c>
@@ -9876,11 +9544,8 @@
       <c r="F91" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="G91" t="s">
-        <v>1132</v>
-      </c>
-    </row>
-    <row r="92" spans="1:7" ht="39">
+    </row>
+    <row r="92" spans="1:6" ht="39">
       <c r="A92" s="6" t="s">
         <v>374</v>
       </c>
@@ -9899,11 +9564,8 @@
       <c r="F92" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="G92" t="s">
-        <v>1132</v>
-      </c>
-    </row>
-    <row r="93" spans="1:7" ht="91">
+    </row>
+    <row r="93" spans="1:6" ht="91">
       <c r="A93" s="6" t="s">
         <v>378</v>
       </c>
@@ -9922,11 +9584,8 @@
       <c r="F93" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="G93" t="s">
-        <v>1132</v>
-      </c>
-    </row>
-    <row r="94" spans="1:7" ht="39">
+    </row>
+    <row r="94" spans="1:6" ht="39">
       <c r="A94" s="6" t="s">
         <v>382</v>
       </c>
@@ -9945,11 +9604,8 @@
       <c r="F94" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G94" t="s">
-        <v>1132</v>
-      </c>
-    </row>
-    <row r="95" spans="1:7" ht="130">
+    </row>
+    <row r="95" spans="1:6" ht="130">
       <c r="A95" s="6" t="s">
         <v>387</v>
       </c>
@@ -9968,11 +9624,8 @@
       <c r="F95" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="G95" t="s">
-        <v>1132</v>
-      </c>
-    </row>
-    <row r="96" spans="1:7" ht="65">
+    </row>
+    <row r="96" spans="1:6" ht="65">
       <c r="A96" s="6" t="s">
         <v>391</v>
       </c>
@@ -9991,11 +9644,8 @@
       <c r="F96" s="6" t="s">
         <v>396</v>
       </c>
-      <c r="G96" t="s">
-        <v>1132</v>
-      </c>
-    </row>
-    <row r="97" spans="1:7" ht="52">
+    </row>
+    <row r="97" spans="1:6" ht="52">
       <c r="A97" s="6" t="s">
         <v>397</v>
       </c>
@@ -10014,11 +9664,8 @@
       <c r="F97" s="6" t="s">
         <v>396</v>
       </c>
-      <c r="G97" t="s">
-        <v>1132</v>
-      </c>
-    </row>
-    <row r="98" spans="1:7" ht="78">
+    </row>
+    <row r="98" spans="1:6" ht="78">
       <c r="A98" s="6" t="s">
         <v>400</v>
       </c>
@@ -10037,11 +9684,8 @@
       <c r="F98" s="6" t="s">
         <v>396</v>
       </c>
-      <c r="G98" t="s">
-        <v>1132</v>
-      </c>
-    </row>
-    <row r="99" spans="1:7" ht="39">
+    </row>
+    <row r="99" spans="1:6" ht="39">
       <c r="A99" s="6" t="s">
         <v>404</v>
       </c>
@@ -10060,11 +9704,8 @@
       <c r="F99" s="6" t="s">
         <v>396</v>
       </c>
-      <c r="G99" t="s">
-        <v>1132</v>
-      </c>
-    </row>
-    <row r="100" spans="1:7" ht="65">
+    </row>
+    <row r="100" spans="1:6" ht="65">
       <c r="A100" s="6" t="s">
         <v>407</v>
       </c>
@@ -10083,11 +9724,8 @@
       <c r="F100" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="G100" t="s">
-        <v>1132</v>
-      </c>
-    </row>
-    <row r="101" spans="1:7" ht="130">
+    </row>
+    <row r="101" spans="1:6" ht="130">
       <c r="A101" s="6" t="s">
         <v>412</v>
       </c>
@@ -10106,11 +9744,8 @@
       <c r="F101" s="6" t="s">
         <v>309</v>
       </c>
-      <c r="G101" t="s">
-        <v>1132</v>
-      </c>
-    </row>
-    <row r="102" spans="1:7" ht="117">
+    </row>
+    <row r="102" spans="1:6" ht="117">
       <c r="A102" s="6" t="s">
         <v>417</v>
       </c>
@@ -10129,11 +9764,8 @@
       <c r="F102" s="6" t="s">
         <v>309</v>
       </c>
-      <c r="G102" t="s">
-        <v>1132</v>
-      </c>
-    </row>
-    <row r="103" spans="1:7" ht="78">
+    </row>
+    <row r="103" spans="1:6" ht="78">
       <c r="A103" s="6" t="s">
         <v>421</v>
       </c>
@@ -10152,11 +9784,8 @@
       <c r="F103" s="6" t="s">
         <v>309</v>
       </c>
-      <c r="G103" t="s">
-        <v>1132</v>
-      </c>
-    </row>
-    <row r="104" spans="1:7" ht="130">
+    </row>
+    <row r="104" spans="1:6" ht="130">
       <c r="A104" s="6" t="s">
         <v>425</v>
       </c>
@@ -10175,11 +9804,8 @@
       <c r="F104" s="6" t="s">
         <v>309</v>
       </c>
-      <c r="G104" t="s">
-        <v>1132</v>
-      </c>
-    </row>
-    <row r="105" spans="1:7" ht="39">
+    </row>
+    <row r="105" spans="1:6" ht="39">
       <c r="A105" s="6" t="s">
         <v>429</v>
       </c>
@@ -10198,11 +9824,8 @@
       <c r="F105" s="6" t="s">
         <v>309</v>
       </c>
-      <c r="G105" t="s">
-        <v>1132</v>
-      </c>
-    </row>
-    <row r="106" spans="1:7" ht="39">
+    </row>
+    <row r="106" spans="1:6" ht="39">
       <c r="A106" s="6" t="s">
         <v>433</v>
       </c>
@@ -10221,11 +9844,8 @@
       <c r="F106" s="6" t="s">
         <v>309</v>
       </c>
-      <c r="G106" t="s">
-        <v>1132</v>
-      </c>
-    </row>
-    <row r="107" spans="1:7" ht="39">
+    </row>
+    <row r="107" spans="1:6" ht="39">
       <c r="A107" s="6" t="s">
         <v>437</v>
       </c>
@@ -10244,11 +9864,8 @@
       <c r="F107" s="6" t="s">
         <v>309</v>
       </c>
-      <c r="G107" t="s">
-        <v>1132</v>
-      </c>
-    </row>
-    <row r="108" spans="1:7" ht="65">
+    </row>
+    <row r="108" spans="1:6" ht="65">
       <c r="A108" s="6" t="s">
         <v>441</v>
       </c>
@@ -10267,11 +9884,8 @@
       <c r="F108" s="6" t="s">
         <v>309</v>
       </c>
-      <c r="G108" t="s">
-        <v>1132</v>
-      </c>
-    </row>
-    <row r="109" spans="1:7" ht="39">
+    </row>
+    <row r="109" spans="1:6" ht="39">
       <c r="A109" s="6" t="s">
         <v>446</v>
       </c>
@@ -10290,11 +9904,8 @@
       <c r="F109" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="G109" t="s">
-        <v>1132</v>
-      </c>
-    </row>
-    <row r="110" spans="1:7" ht="52">
+    </row>
+    <row r="110" spans="1:6" ht="52">
       <c r="A110" s="6" t="s">
         <v>451</v>
       </c>
@@ -10313,11 +9924,8 @@
       <c r="F110" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="G110" t="s">
-        <v>1132</v>
-      </c>
-    </row>
-    <row r="111" spans="1:7" ht="65">
+    </row>
+    <row r="111" spans="1:6" ht="65">
       <c r="A111" s="6" t="s">
         <v>454</v>
       </c>
@@ -10336,11 +9944,8 @@
       <c r="F111" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="G111" t="s">
-        <v>1132</v>
-      </c>
-    </row>
-    <row r="112" spans="1:7" ht="39">
+    </row>
+    <row r="112" spans="1:6" ht="39">
       <c r="A112" s="6" t="s">
         <v>458</v>
       </c>
@@ -10359,11 +9964,8 @@
       <c r="F112" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="G112" t="s">
-        <v>1132</v>
-      </c>
-    </row>
-    <row r="113" spans="1:7" ht="130">
+    </row>
+    <row r="113" spans="1:6" ht="130">
       <c r="A113" s="6" t="s">
         <v>461</v>
       </c>
@@ -10382,11 +9984,8 @@
       <c r="F113" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="G113" t="s">
-        <v>1132</v>
-      </c>
-    </row>
-    <row r="114" spans="1:7" ht="91">
+    </row>
+    <row r="114" spans="1:6" ht="91">
       <c r="A114" s="6" t="s">
         <v>465</v>
       </c>
@@ -10405,11 +10004,8 @@
       <c r="F114" s="6" t="s">
         <v>470</v>
       </c>
-      <c r="G114" t="s">
-        <v>1132</v>
-      </c>
-    </row>
-    <row r="115" spans="1:7" ht="52">
+    </row>
+    <row r="115" spans="1:6" ht="52">
       <c r="A115" s="6" t="s">
         <v>471</v>
       </c>
@@ -10428,11 +10024,8 @@
       <c r="F115" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G115" t="s">
-        <v>1132</v>
-      </c>
-    </row>
-    <row r="116" spans="1:7" ht="39" hidden="1">
+    </row>
+    <row r="116" spans="1:6" ht="39">
       <c r="A116" s="6" t="s">
         <v>475</v>
       </c>
@@ -10451,11 +10044,8 @@
       <c r="F116" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G116" t="s">
-        <v>1131</v>
-      </c>
-    </row>
-    <row r="117" spans="1:7" ht="39">
+    </row>
+    <row r="117" spans="1:6" ht="39">
       <c r="A117" s="6" t="s">
         <v>479</v>
       </c>
@@ -10474,11 +10064,8 @@
       <c r="F117" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G117" t="s">
-        <v>1132</v>
-      </c>
-    </row>
-    <row r="118" spans="1:7" ht="26">
+    </row>
+    <row r="118" spans="1:6" ht="26">
       <c r="A118" s="6" t="s">
         <v>483</v>
       </c>
@@ -10497,11 +10084,8 @@
       <c r="F118" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G118" t="s">
-        <v>1132</v>
-      </c>
-    </row>
-    <row r="119" spans="1:7" ht="78">
+    </row>
+    <row r="119" spans="1:6" ht="78">
       <c r="A119" s="6" t="s">
         <v>487</v>
       </c>
@@ -10520,11 +10104,8 @@
       <c r="F119" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G119" t="s">
-        <v>1132</v>
-      </c>
-    </row>
-    <row r="120" spans="1:7" ht="26">
+    </row>
+    <row r="120" spans="1:6" ht="26">
       <c r="A120" s="6" t="s">
         <v>491</v>
       </c>
@@ -10543,11 +10124,8 @@
       <c r="F120" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="G120" t="s">
-        <v>1132</v>
-      </c>
-    </row>
-    <row r="121" spans="1:7" ht="52">
+    </row>
+    <row r="121" spans="1:6" ht="52">
       <c r="A121" s="6" t="s">
         <v>496</v>
       </c>
@@ -10566,11 +10144,8 @@
       <c r="F121" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="G121" t="s">
-        <v>1132</v>
-      </c>
-    </row>
-    <row r="122" spans="1:7" ht="39">
+    </row>
+    <row r="122" spans="1:6" ht="39">
       <c r="A122" s="6" t="s">
         <v>500</v>
       </c>
@@ -10589,11 +10164,8 @@
       <c r="F122" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="G122" t="s">
-        <v>1132</v>
-      </c>
-    </row>
-    <row r="123" spans="1:7" ht="52">
+    </row>
+    <row r="123" spans="1:6" ht="52">
       <c r="A123" s="6" t="s">
         <v>503</v>
       </c>
@@ -10612,11 +10184,8 @@
       <c r="F123" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="G123" t="s">
-        <v>1132</v>
-      </c>
-    </row>
-    <row r="124" spans="1:7" ht="39">
+    </row>
+    <row r="124" spans="1:6" ht="39">
       <c r="A124" s="6" t="s">
         <v>507</v>
       </c>
@@ -10635,11 +10204,8 @@
       <c r="F124" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="G124" t="s">
-        <v>1132</v>
-      </c>
-    </row>
-    <row r="125" spans="1:7" ht="26">
+    </row>
+    <row r="125" spans="1:6" ht="26">
       <c r="A125" s="6" t="s">
         <v>511</v>
       </c>
@@ -10658,11 +10224,8 @@
       <c r="F125" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="G125" t="s">
-        <v>1132</v>
-      </c>
-    </row>
-    <row r="126" spans="1:7" ht="78">
+    </row>
+    <row r="126" spans="1:6" ht="78">
       <c r="A126" s="6" t="s">
         <v>515</v>
       </c>
@@ -10681,11 +10244,8 @@
       <c r="F126" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G126" t="s">
-        <v>1132</v>
-      </c>
-    </row>
-    <row r="127" spans="1:7" ht="91">
+    </row>
+    <row r="127" spans="1:6" ht="91">
       <c r="A127" s="6" t="s">
         <v>520</v>
       </c>
@@ -10704,11 +10264,8 @@
       <c r="F127" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="G127" t="s">
-        <v>1132</v>
-      </c>
-    </row>
-    <row r="128" spans="1:7" ht="39">
+    </row>
+    <row r="128" spans="1:6" ht="39">
       <c r="A128" s="6" t="s">
         <v>525</v>
       </c>
@@ -10727,11 +10284,8 @@
       <c r="F128" s="6" t="s">
         <v>396</v>
       </c>
-      <c r="G128" t="s">
-        <v>1132</v>
-      </c>
-    </row>
-    <row r="129" spans="1:7" ht="39">
+    </row>
+    <row r="129" spans="1:6" ht="39">
       <c r="A129" s="6" t="s">
         <v>529</v>
       </c>
@@ -10750,11 +10304,8 @@
       <c r="F129" s="6" t="s">
         <v>396</v>
       </c>
-      <c r="G129" t="s">
-        <v>1132</v>
-      </c>
-    </row>
-    <row r="130" spans="1:7" ht="78">
+    </row>
+    <row r="130" spans="1:6" ht="78">
       <c r="A130" s="6" t="s">
         <v>533</v>
       </c>
@@ -10773,11 +10324,8 @@
       <c r="F130" s="6" t="s">
         <v>396</v>
       </c>
-      <c r="G130" t="s">
-        <v>1132</v>
-      </c>
-    </row>
-    <row r="131" spans="1:7" ht="39">
+    </row>
+    <row r="131" spans="1:6" ht="39">
       <c r="A131" s="6" t="s">
         <v>537</v>
       </c>
@@ -10796,11 +10344,8 @@
       <c r="F131" s="6" t="s">
         <v>396</v>
       </c>
-      <c r="G131" t="s">
-        <v>1132</v>
-      </c>
-    </row>
-    <row r="132" spans="1:7" ht="52">
+    </row>
+    <row r="132" spans="1:6" ht="52">
       <c r="A132" s="6" t="s">
         <v>541</v>
       </c>
@@ -10819,11 +10364,8 @@
       <c r="F132" s="6" t="s">
         <v>396</v>
       </c>
-      <c r="G132" t="s">
-        <v>1132</v>
-      </c>
-    </row>
-    <row r="133" spans="1:7" ht="52">
+    </row>
+    <row r="133" spans="1:6" ht="52">
       <c r="A133" s="6" t="s">
         <v>544</v>
       </c>
@@ -10842,11 +10384,8 @@
       <c r="F133" s="6" t="s">
         <v>396</v>
       </c>
-      <c r="G133" t="s">
-        <v>1132</v>
-      </c>
-    </row>
-    <row r="134" spans="1:7" ht="39">
+    </row>
+    <row r="134" spans="1:6" ht="39">
       <c r="A134" s="6" t="s">
         <v>548</v>
       </c>
@@ -10865,11 +10404,8 @@
       <c r="F134" s="6" t="s">
         <v>396</v>
       </c>
-      <c r="G134" t="s">
-        <v>1132</v>
-      </c>
-    </row>
-    <row r="135" spans="1:7" ht="26">
+    </row>
+    <row r="135" spans="1:6" ht="26">
       <c r="A135" s="6" t="s">
         <v>551</v>
       </c>
@@ -10888,11 +10424,8 @@
       <c r="F135" s="6" t="s">
         <v>396</v>
       </c>
-      <c r="G135" t="s">
-        <v>1132</v>
-      </c>
-    </row>
-    <row r="136" spans="1:7" ht="52">
+    </row>
+    <row r="136" spans="1:6" ht="52">
       <c r="A136" s="6" t="s">
         <v>555</v>
       </c>
@@ -10911,11 +10444,8 @@
       <c r="F136" s="6" t="s">
         <v>396</v>
       </c>
-      <c r="G136" t="s">
-        <v>1132</v>
-      </c>
-    </row>
-    <row r="137" spans="1:7" ht="52" hidden="1">
+    </row>
+    <row r="137" spans="1:6" ht="52">
       <c r="A137" s="6" t="s">
         <v>560</v>
       </c>
@@ -10934,11 +10464,8 @@
       <c r="F137" s="6" t="s">
         <v>396</v>
       </c>
-      <c r="G137" t="s">
-        <v>1131</v>
-      </c>
-    </row>
-    <row r="138" spans="1:7" ht="65">
+    </row>
+    <row r="138" spans="1:6" ht="65">
       <c r="A138" s="6" t="s">
         <v>564</v>
       </c>
@@ -10957,11 +10484,8 @@
       <c r="F138" s="6" t="s">
         <v>396</v>
       </c>
-      <c r="G138" t="s">
-        <v>1132</v>
-      </c>
-    </row>
-    <row r="139" spans="1:7" ht="52" hidden="1">
+    </row>
+    <row r="139" spans="1:6" ht="52">
       <c r="A139" s="6" t="s">
         <v>568</v>
       </c>
@@ -10980,11 +10504,8 @@
       <c r="F139" s="6" t="s">
         <v>396</v>
       </c>
-      <c r="G139" t="s">
-        <v>1131</v>
-      </c>
-    </row>
-    <row r="140" spans="1:7" ht="52">
+    </row>
+    <row r="140" spans="1:6" ht="52">
       <c r="A140" s="6" t="s">
         <v>571</v>
       </c>
@@ -11003,11 +10524,8 @@
       <c r="F140" s="6" t="s">
         <v>396</v>
       </c>
-      <c r="G140" t="s">
-        <v>1132</v>
-      </c>
-    </row>
-    <row r="141" spans="1:7" ht="39">
+    </row>
+    <row r="141" spans="1:6" ht="39">
       <c r="A141" s="6" t="s">
         <v>576</v>
       </c>
@@ -11026,11 +10544,8 @@
       <c r="F141" s="6" t="s">
         <v>396</v>
       </c>
-      <c r="G141" t="s">
-        <v>1132</v>
-      </c>
-    </row>
-    <row r="142" spans="1:7" ht="52">
+    </row>
+    <row r="142" spans="1:6" ht="52">
       <c r="A142" s="6" t="s">
         <v>581</v>
       </c>
@@ -11049,11 +10564,8 @@
       <c r="F142" s="6" t="s">
         <v>396</v>
       </c>
-      <c r="G142" t="s">
-        <v>1132</v>
-      </c>
-    </row>
-    <row r="143" spans="1:7" ht="39">
+    </row>
+    <row r="143" spans="1:6" ht="39">
       <c r="A143" s="6" t="s">
         <v>585</v>
       </c>
@@ -11072,11 +10584,8 @@
       <c r="F143" s="6" t="s">
         <v>396</v>
       </c>
-      <c r="G143" t="s">
-        <v>1132</v>
-      </c>
-    </row>
-    <row r="144" spans="1:7" ht="78">
+    </row>
+    <row r="144" spans="1:6" ht="78">
       <c r="A144" s="6" t="s">
         <v>588</v>
       </c>
@@ -11095,11 +10604,8 @@
       <c r="F144" s="6" t="s">
         <v>396</v>
       </c>
-      <c r="G144" t="s">
-        <v>1132</v>
-      </c>
-    </row>
-    <row r="145" spans="1:7" ht="91">
+    </row>
+    <row r="145" spans="1:6" ht="91">
       <c r="A145" s="6" t="s">
         <v>592</v>
       </c>
@@ -11118,11 +10624,8 @@
       <c r="F145" s="6" t="s">
         <v>396</v>
       </c>
-      <c r="G145" t="s">
-        <v>1132</v>
-      </c>
-    </row>
-    <row r="146" spans="1:7" ht="39">
+    </row>
+    <row r="146" spans="1:6" ht="39">
       <c r="A146" s="6" t="s">
         <v>596</v>
       </c>
@@ -11141,11 +10644,8 @@
       <c r="F146" s="6" t="s">
         <v>396</v>
       </c>
-      <c r="G146" t="s">
-        <v>1132</v>
-      </c>
-    </row>
-    <row r="147" spans="1:7" ht="39">
+    </row>
+    <row r="147" spans="1:6" ht="39">
       <c r="A147" s="6" t="s">
         <v>600</v>
       </c>
@@ -11164,11 +10664,8 @@
       <c r="F147" s="6" t="s">
         <v>396</v>
       </c>
-      <c r="G147" t="s">
-        <v>1132</v>
-      </c>
-    </row>
-    <row r="148" spans="1:7" ht="26" hidden="1">
+    </row>
+    <row r="148" spans="1:6" ht="26">
       <c r="A148" s="6" t="s">
         <v>604</v>
       </c>
@@ -11187,11 +10684,8 @@
       <c r="F148" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="G148" t="s">
-        <v>1131</v>
-      </c>
-    </row>
-    <row r="149" spans="1:7" ht="52" hidden="1">
+    </row>
+    <row r="149" spans="1:6" ht="52">
       <c r="A149" s="6" t="s">
         <v>609</v>
       </c>
@@ -11210,11 +10704,8 @@
       <c r="F149" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="G149" t="s">
-        <v>1131</v>
-      </c>
-    </row>
-    <row r="150" spans="1:7" ht="39" hidden="1">
+    </row>
+    <row r="150" spans="1:6" ht="39">
       <c r="A150" s="6" t="s">
         <v>613</v>
       </c>
@@ -11233,11 +10724,8 @@
       <c r="F150" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="G150" t="s">
-        <v>1131</v>
-      </c>
-    </row>
-    <row r="151" spans="1:7" ht="39" hidden="1">
+    </row>
+    <row r="151" spans="1:6" ht="39">
       <c r="A151" s="6" t="s">
         <v>617</v>
       </c>
@@ -11256,11 +10744,8 @@
       <c r="F151" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="G151" t="s">
-        <v>1131</v>
-      </c>
-    </row>
-    <row r="152" spans="1:7" ht="26" hidden="1">
+    </row>
+    <row r="152" spans="1:6" ht="26">
       <c r="A152" s="6" t="s">
         <v>621</v>
       </c>
@@ -11279,11 +10764,8 @@
       <c r="F152" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="G152" t="s">
-        <v>1131</v>
-      </c>
-    </row>
-    <row r="153" spans="1:7" ht="26" hidden="1">
+    </row>
+    <row r="153" spans="1:6" ht="26">
       <c r="A153" s="6" t="s">
         <v>625</v>
       </c>
@@ -11302,11 +10784,8 @@
       <c r="F153" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="G153" t="s">
-        <v>1131</v>
-      </c>
-    </row>
-    <row r="154" spans="1:7" ht="52" hidden="1">
+    </row>
+    <row r="154" spans="1:6" ht="52">
       <c r="A154" s="6" t="s">
         <v>629</v>
       </c>
@@ -11325,11 +10804,8 @@
       <c r="F154" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="G154" t="s">
-        <v>1131</v>
-      </c>
-    </row>
-    <row r="155" spans="1:7" ht="52" hidden="1">
+    </row>
+    <row r="155" spans="1:6" ht="52">
       <c r="A155" s="6" t="s">
         <v>633</v>
       </c>
@@ -11348,11 +10824,8 @@
       <c r="F155" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="G155" t="s">
-        <v>1131</v>
-      </c>
-    </row>
-    <row r="156" spans="1:7" ht="52">
+    </row>
+    <row r="156" spans="1:6" ht="52">
       <c r="A156" s="6" t="s">
         <v>636</v>
       </c>
@@ -11371,11 +10844,8 @@
       <c r="F156" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="G156" t="s">
-        <v>1132</v>
-      </c>
-    </row>
-    <row r="157" spans="1:7" ht="65">
+    </row>
+    <row r="157" spans="1:6" ht="65">
       <c r="A157" s="6" t="s">
         <v>640</v>
       </c>
@@ -11394,11 +10864,8 @@
       <c r="F157" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G157" t="s">
-        <v>1132</v>
-      </c>
-    </row>
-    <row r="158" spans="1:7" ht="39">
+    </row>
+    <row r="158" spans="1:6" ht="39">
       <c r="A158" s="6" t="s">
         <v>645</v>
       </c>
@@ -11417,11 +10884,8 @@
       <c r="F158" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G158" t="s">
-        <v>1132</v>
-      </c>
-    </row>
-    <row r="159" spans="1:7" ht="52">
+    </row>
+    <row r="159" spans="1:6" ht="52">
       <c r="A159" s="6" t="s">
         <v>649</v>
       </c>
@@ -11440,11 +10904,8 @@
       <c r="F159" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="G159" t="s">
-        <v>1132</v>
-      </c>
-    </row>
-    <row r="160" spans="1:7" ht="104">
+    </row>
+    <row r="160" spans="1:6" ht="104">
       <c r="A160" s="6" t="s">
         <v>653</v>
       </c>
@@ -11463,11 +10924,8 @@
       <c r="F160" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="G160" t="s">
-        <v>1132</v>
-      </c>
-    </row>
-    <row r="161" spans="1:7" ht="52">
+    </row>
+    <row r="161" spans="1:6" ht="52">
       <c r="A161" s="6" t="s">
         <v>657</v>
       </c>
@@ -11486,11 +10944,8 @@
       <c r="F161" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="G161" t="s">
-        <v>1132</v>
-      </c>
-    </row>
-    <row r="162" spans="1:7" ht="65">
+    </row>
+    <row r="162" spans="1:6" ht="65">
       <c r="A162" s="6" t="s">
         <v>661</v>
       </c>
@@ -11509,11 +10964,8 @@
       <c r="F162" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="G162" t="s">
-        <v>1132</v>
-      </c>
-    </row>
-    <row r="163" spans="1:7" ht="39">
+    </row>
+    <row r="163" spans="1:6" ht="39">
       <c r="A163" s="6" t="s">
         <v>665</v>
       </c>
@@ -11532,11 +10984,8 @@
       <c r="F163" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="G163" t="s">
-        <v>1132</v>
-      </c>
-    </row>
-    <row r="164" spans="1:7" ht="91" hidden="1">
+    </row>
+    <row r="164" spans="1:6" ht="91">
       <c r="A164" s="6" t="s">
         <v>669</v>
       </c>
@@ -11555,11 +11004,8 @@
       <c r="F164" s="6" t="s">
         <v>326</v>
       </c>
-      <c r="G164" t="s">
-        <v>1131</v>
-      </c>
-    </row>
-    <row r="165" spans="1:7" ht="52">
+    </row>
+    <row r="165" spans="1:6" ht="52">
       <c r="A165" s="6" t="s">
         <v>673</v>
       </c>
@@ -11578,11 +11024,8 @@
       <c r="F165" s="6" t="s">
         <v>470</v>
       </c>
-      <c r="G165" t="s">
-        <v>1132</v>
-      </c>
-    </row>
-    <row r="166" spans="1:7" ht="65">
+    </row>
+    <row r="166" spans="1:6" ht="65">
       <c r="A166" s="6" t="s">
         <v>678</v>
       </c>
@@ -11601,11 +11044,8 @@
       <c r="F166" s="6" t="s">
         <v>470</v>
       </c>
-      <c r="G166" t="s">
-        <v>1132</v>
-      </c>
-    </row>
-    <row r="167" spans="1:7" ht="65">
+    </row>
+    <row r="167" spans="1:6" ht="65">
       <c r="A167" s="6" t="s">
         <v>682</v>
       </c>
@@ -11624,11 +11064,8 @@
       <c r="F167" s="6" t="s">
         <v>470</v>
       </c>
-      <c r="G167" t="s">
-        <v>1132</v>
-      </c>
-    </row>
-    <row r="168" spans="1:7" ht="39">
+    </row>
+    <row r="168" spans="1:6" ht="39">
       <c r="A168" s="6" t="s">
         <v>686</v>
       </c>
@@ -11647,11 +11084,8 @@
       <c r="F168" s="6" t="s">
         <v>470</v>
       </c>
-      <c r="G168" t="s">
-        <v>1132</v>
-      </c>
-    </row>
-    <row r="169" spans="1:7" ht="26">
+    </row>
+    <row r="169" spans="1:6" ht="26">
       <c r="A169" s="6" t="s">
         <v>690</v>
       </c>
@@ -11670,11 +11104,8 @@
       <c r="F169" s="6" t="s">
         <v>470</v>
       </c>
-      <c r="G169" t="s">
-        <v>1132</v>
-      </c>
-    </row>
-    <row r="170" spans="1:7" ht="52">
+    </row>
+    <row r="170" spans="1:6" ht="52">
       <c r="A170" s="6" t="s">
         <v>695</v>
       </c>
@@ -11693,11 +11124,8 @@
       <c r="F170" s="6" t="s">
         <v>470</v>
       </c>
-      <c r="G170" t="s">
-        <v>1132</v>
-      </c>
-    </row>
-    <row r="171" spans="1:7" ht="65">
+    </row>
+    <row r="171" spans="1:6" ht="65">
       <c r="A171" s="6" t="s">
         <v>698</v>
       </c>
@@ -11716,11 +11144,8 @@
       <c r="F171" s="6" t="s">
         <v>470</v>
       </c>
-      <c r="G171" t="s">
-        <v>1132</v>
-      </c>
-    </row>
-    <row r="172" spans="1:7" ht="26">
+    </row>
+    <row r="172" spans="1:6" ht="26">
       <c r="A172" s="6" t="s">
         <v>701</v>
       </c>
@@ -11739,11 +11164,8 @@
       <c r="F172" s="6" t="s">
         <v>304</v>
       </c>
-      <c r="G172" t="s">
-        <v>1132</v>
-      </c>
-    </row>
-    <row r="173" spans="1:7" ht="52">
+    </row>
+    <row r="173" spans="1:6" ht="52">
       <c r="A173" s="6" t="s">
         <v>706</v>
       </c>
@@ -11762,11 +11184,8 @@
       <c r="F173" s="6" t="s">
         <v>304</v>
       </c>
-      <c r="G173" t="s">
-        <v>1132</v>
-      </c>
-    </row>
-    <row r="174" spans="1:7" ht="104">
+    </row>
+    <row r="174" spans="1:6" ht="104">
       <c r="A174" s="6" t="s">
         <v>709</v>
       </c>
@@ -11785,11 +11204,8 @@
       <c r="F174" s="6" t="s">
         <v>309</v>
       </c>
-      <c r="G174" t="s">
-        <v>1132</v>
-      </c>
-    </row>
-    <row r="175" spans="1:7" ht="91">
+    </row>
+    <row r="175" spans="1:6" ht="91">
       <c r="A175" s="6" t="s">
         <v>714</v>
       </c>
@@ -11808,11 +11224,8 @@
       <c r="F175" s="6" t="s">
         <v>309</v>
       </c>
-      <c r="G175" t="s">
-        <v>1132</v>
-      </c>
-    </row>
-    <row r="176" spans="1:7" ht="91">
+    </row>
+    <row r="176" spans="1:6" ht="91">
       <c r="A176" s="6" t="s">
         <v>718</v>
       </c>
@@ -11831,11 +11244,8 @@
       <c r="F176" s="6" t="s">
         <v>309</v>
       </c>
-      <c r="G176" t="s">
-        <v>1132</v>
-      </c>
-    </row>
-    <row r="177" spans="1:7" ht="65">
+    </row>
+    <row r="177" spans="1:6" ht="65">
       <c r="A177" s="6" t="s">
         <v>722</v>
       </c>
@@ -11854,11 +11264,8 @@
       <c r="F177" s="6" t="s">
         <v>309</v>
       </c>
-      <c r="G177" t="s">
-        <v>1132</v>
-      </c>
-    </row>
-    <row r="178" spans="1:7" ht="52" hidden="1">
+    </row>
+    <row r="178" spans="1:6" ht="52">
       <c r="A178" s="6" t="s">
         <v>726</v>
       </c>
@@ -11877,11 +11284,8 @@
       <c r="F178" s="6" t="s">
         <v>309</v>
       </c>
-      <c r="G178" t="s">
-        <v>1131</v>
-      </c>
-    </row>
-    <row r="179" spans="1:7" ht="78">
+    </row>
+    <row r="179" spans="1:6" ht="78">
       <c r="A179" s="6" t="s">
         <v>729</v>
       </c>
@@ -11900,11 +11304,8 @@
       <c r="F179" s="6" t="s">
         <v>309</v>
       </c>
-      <c r="G179" t="s">
-        <v>1132</v>
-      </c>
-    </row>
-    <row r="180" spans="1:7" ht="52">
+    </row>
+    <row r="180" spans="1:6" ht="52">
       <c r="A180" s="6" t="s">
         <v>733</v>
       </c>
@@ -11923,11 +11324,8 @@
       <c r="F180" s="6" t="s">
         <v>309</v>
       </c>
-      <c r="G180" t="s">
-        <v>1132</v>
-      </c>
-    </row>
-    <row r="181" spans="1:7" ht="52">
+    </row>
+    <row r="181" spans="1:6" ht="52">
       <c r="A181" s="6" t="s">
         <v>737</v>
       </c>
@@ -11946,11 +11344,8 @@
       <c r="F181" s="6" t="s">
         <v>309</v>
       </c>
-      <c r="G181" t="s">
-        <v>1132</v>
-      </c>
-    </row>
-    <row r="182" spans="1:7" ht="104">
+    </row>
+    <row r="182" spans="1:6" ht="104">
       <c r="A182" s="6" t="s">
         <v>741</v>
       </c>
@@ -11969,11 +11364,8 @@
       <c r="F182" s="6" t="s">
         <v>309</v>
       </c>
-      <c r="G182" t="s">
-        <v>1132</v>
-      </c>
-    </row>
-    <row r="183" spans="1:7" ht="78">
+    </row>
+    <row r="183" spans="1:6" ht="78">
       <c r="A183" s="6" t="s">
         <v>745</v>
       </c>
@@ -11992,11 +11384,8 @@
       <c r="F183" s="6" t="s">
         <v>309</v>
       </c>
-      <c r="G183" t="s">
-        <v>1132</v>
-      </c>
-    </row>
-    <row r="184" spans="1:7" ht="65">
+    </row>
+    <row r="184" spans="1:6" ht="65">
       <c r="A184" s="6" t="s">
         <v>750</v>
       </c>
@@ -12015,11 +11404,8 @@
       <c r="F184" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G184" t="s">
-        <v>1132</v>
-      </c>
-    </row>
-    <row r="185" spans="1:7" ht="52">
+    </row>
+    <row r="185" spans="1:6" ht="52">
       <c r="A185" s="6" t="s">
         <v>755</v>
       </c>
@@ -12038,11 +11424,8 @@
       <c r="F185" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G185" t="s">
-        <v>1132</v>
-      </c>
-    </row>
-    <row r="186" spans="1:7" ht="52">
+    </row>
+    <row r="186" spans="1:6" ht="52">
       <c r="A186" s="6" t="s">
         <v>759</v>
       </c>
@@ -12061,11 +11444,8 @@
       <c r="F186" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G186" t="s">
-        <v>1132</v>
-      </c>
-    </row>
-    <row r="187" spans="1:7" ht="39">
+    </row>
+    <row r="187" spans="1:6" ht="39">
       <c r="A187" s="6" t="s">
         <v>763</v>
       </c>
@@ -12084,11 +11464,8 @@
       <c r="F187" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G187" t="s">
-        <v>1132</v>
-      </c>
-    </row>
-    <row r="188" spans="1:7" ht="65">
+    </row>
+    <row r="188" spans="1:6" ht="65">
       <c r="A188" s="6" t="s">
         <v>767</v>
       </c>
@@ -12107,11 +11484,8 @@
       <c r="F188" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G188" t="s">
-        <v>1132</v>
-      </c>
-    </row>
-    <row r="189" spans="1:7" ht="65">
+    </row>
+    <row r="189" spans="1:6" ht="65">
       <c r="A189" s="6" t="s">
         <v>770</v>
       </c>
@@ -12130,11 +11504,8 @@
       <c r="F189" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="G189" t="s">
-        <v>1132</v>
-      </c>
-    </row>
-    <row r="190" spans="1:7" ht="78">
+    </row>
+    <row r="190" spans="1:6" ht="78">
       <c r="A190" s="6" t="s">
         <v>774</v>
       </c>
@@ -12153,11 +11524,8 @@
       <c r="F190" s="6" t="s">
         <v>309</v>
       </c>
-      <c r="G190" t="s">
-        <v>1132</v>
-      </c>
-    </row>
-    <row r="191" spans="1:7" ht="91">
+    </row>
+    <row r="191" spans="1:6" ht="91">
       <c r="A191" s="6" t="s">
         <v>778</v>
       </c>
@@ -12176,18 +11544,8 @@
       <c r="F191" s="6" t="s">
         <v>146</v>
       </c>
-      <c r="G191" t="s">
-        <v>1132</v>
-      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G191">
-    <filterColumn colId="6">
-      <filters>
-        <filter val="未开放-5.8"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>